<commit_message>
添加 branch -v -vv
</commit_message>
<xml_diff>
--- a/git_cmd.xlsx
+++ b/git_cmd.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9207E2D-520E-4F95-8F65-6E1CEA472E46}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3417239-A692-463E-825C-FC58D4AC1D32}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,7 +311,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>git branch -a 包括远程仓的分支</t>
+    <t>git branch -a 包括远程仓的分支
+-v(-vv) 分支(远程仓分支)信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -839,14 +840,14 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" ht="19.95" customHeight="1">
+    <row r="15" spans="1:3" ht="27.6">
       <c r="A15" t="s">
         <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>